<commit_message>
Retrieve all negative data for one sheet
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -14,30 +14,76 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+  <si>
+    <t>1: must
+(if POS content management tool is available in the market)</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Marketing Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; visual check </t>
+  </si>
+  <si>
+    <t>Is the most actual content is shown on all digital devices? (if not used by customers or sales personnel for individual product presentation)</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Audit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (if POS content management tool is available in the market)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The importer ensures that only the most actual content is shown on all digital devices.
+</t>
+  </si>
+  <si>
+    <t>9.7</t>
+  </si>
+  <si>
+    <t>Digital Content-management</t>
+  </si>
+  <si>
+    <t>1: must 
+(if Regional Office offers POS Communication)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; check of orders/deliveries </t>
+  </si>
+  <si>
+    <t>Is the material provided for launches (POS) ordered in time?</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Regional Office or Importer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The importer orders the material provided for launches (Point of Sale (POS) Launch Kit) and other material for further product/technology or seasonal related topics in time and implements this in accordance with BMW Regional Office specifications.
+</t>
+  </si>
+  <si>
+    <t>9.3</t>
+  </si>
+  <si>
+    <t>POS Communication</t>
+  </si>
   <si>
     <t>1: must</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Marketing Manager</t>
-  </si>
-  <si>
     <t>&gt; check of documentation: photographs, letters, ads</t>
   </si>
   <si>
     <t>Is there a documentation for at least one customer event in the last 12 months?</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Audit</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
   <si>
     <t>The content of the launch event is defined by the Regional Office (e.g. by event guidelines)</t>
@@ -448,54 +494,258 @@
     <row r="20"/>
     <row r="21">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27"/>
     <row r="28">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29"/>
     <row r="30">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37">
+      <c r="A37" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="38"/>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40"/>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42"/>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44"/>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46"/>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48"/>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50"/>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52"/>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70"/>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72"/>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74"/>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76"/>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78"/>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="80"/>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82"/>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84"/>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91"/>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="93"/>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creating code for all sheets
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -14,90 +14,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
-  <si>
-    <t>1: must
-(if POS content management tool is available in the market)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+  <si>
+    <t>1: must</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
-    <t>Marketing Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt; visual check </t>
-  </si>
-  <si>
-    <t>Is the most actual content is shown on all digital devices? (if not used by customers or sales personnel for individual product presentation)</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
-    <t>Audit</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (if POS content management tool is available in the market)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The importer ensures that only the most actual content is shown on all digital devices.
+    <t>Mystery shopping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The importer actively encourages to every prospective customer a test drive after the need analysis and before signing contract. 
 </t>
   </si>
   <si>
-    <t>9.7</t>
-  </si>
-  <si>
-    <t>Digital Content-management</t>
-  </si>
-  <si>
-    <t>1: must 
-(if Regional Office offers POS Communication)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt; check of orders/deliveries </t>
-  </si>
-  <si>
-    <t>Is the material provided for launches (POS) ordered in time?</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Regional Office or Importer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The importer orders the material provided for launches (Point of Sale (POS) Launch Kit) and other material for further product/technology or seasonal related topics in time and implements this in accordance with BMW Regional Office specifications.
-</t>
-  </si>
-  <si>
-    <t>9.3</t>
-  </si>
-  <si>
-    <t>POS Communication</t>
-  </si>
-  <si>
-    <t>1: must</t>
-  </si>
-  <si>
-    <t>&gt; check of documentation: photographs, letters, ads</t>
-  </si>
-  <si>
-    <t>Is there a documentation for at least one customer event in the last 12 months?</t>
-  </si>
-  <si>
-    <t>The content of the launch event is defined by the Regional Office (e.g. by event guidelines)</t>
-  </si>
-  <si>
-    <t>The importer conducts at least one customer event (e.g. VIP event, public or other target group events). 
-In addition to this, the importer conducts at least one event per year covering further launch/product/technology or seasonal related topics. 
-The importer documents all events e.g. by photographs, letters, ads.</t>
-  </si>
-  <si>
-    <t>9.2</t>
-  </si>
-  <si>
-    <t>Events</t>
+    <t>8.4</t>
+  </si>
+  <si>
+    <t>Test Drive Offer</t>
   </si>
 </sst>
 </file>
@@ -462,290 +400,70 @@
       </c>
     </row>
     <row r="10"/>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="11"/>
     <row r="12"/>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-    </row>
+    <row r="13"/>
     <row r="14"/>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-    </row>
+    <row r="15"/>
     <row r="16"/>
     <row r="17">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18"/>
     <row r="19">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20"/>
     <row r="21">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27"/>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>7</v>
-      </c>
-    </row>
+    <row r="28"/>
     <row r="29"/>
     <row r="30">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38"/>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40"/>
-    <row r="41">
-      <c r="A41" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42"/>
-    <row r="43">
-      <c r="A43" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44"/>
-    <row r="45">
-      <c r="A45" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46"/>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48"/>
-    <row r="49">
-      <c r="A49" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="50"/>
-    <row r="51">
-      <c r="A51" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52"/>
-    <row r="53">
-      <c r="A53" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59"/>
-    <row r="60"/>
-    <row r="61"/>
-    <row r="62">
-      <c r="A62" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="65"/>
-    <row r="66"/>
-    <row r="67"/>
-    <row r="68"/>
-    <row r="69">
-      <c r="A69" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="70"/>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72"/>
-    <row r="73">
-      <c r="A73" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74"/>
-    <row r="75">
-      <c r="A75" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76"/>
-    <row r="77">
-      <c r="A77" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="78"/>
-    <row r="79">
-      <c r="A79" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="80"/>
-    <row r="81">
-      <c r="A81" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="82"/>
-    <row r="83">
-      <c r="A83" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="84"/>
-    <row r="85">
-      <c r="A85" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="91"/>
-    <row r="92">
-      <c r="A92" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="93"/>
-    <row r="94">
-      <c r="A94" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>